<commit_message>
corrected Conditionally clear cells in XLSX templates
</commit_message>
<xml_diff>
--- a/source/_static/files/document-generation/demos/conditionally-clear-cells-template.xlsx
+++ b/source/_static/files/document-generation/demos/conditionally-clear-cells-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PlumsailGit\TemplaterTest\Templater\bin\Debug\net461\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{68E69BE7-0B6D-4CC1-B158-F7BBC5A92F4E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="10_ncr:100000_{68E69BE7-0B6D-4CC1-B158-F7BBC5A92F4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{D28C8233-CD5B-4A18-8C9B-6DE80ABA2AF8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{2A8C93E8-18E1-47EF-BD03-E7FC040C7E6E}"/>
   </bookViews>
@@ -18,10 +18,15 @@
   <definedNames>
     <definedName name="ConfidentialityNotice">Sheet1!$A$9:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,38 +38,38 @@
     <t>Company details</t>
   </si>
   <si>
+    <t>Company name:</t>
+  </si>
+  <si>
     <t>{{companyName}}</t>
   </si>
   <si>
+    <t>Site:</t>
+  </si>
+  <si>
     <t>{{site}}</t>
   </si>
   <si>
-    <t>Company name:</t>
-  </si>
-  <si>
-    <t>Site:</t>
-  </si>
-  <si>
-    <t>{{contacts.address}} {{contacts}:collapse:hide}</t>
-  </si>
-  <si>
-    <t>Contacts {{contacts}:collapse:hide}</t>
-  </si>
-  <si>
-    <t>{{contacts.phoneNumber}} {{contacts}:collapse:hide}</t>
+    <t>Contacts {{contacts}:hide-block-if-empty}</t>
+  </si>
+  <si>
+    <t>{{contacts.address}} {{contacts}:hide-block-if-empty}</t>
+  </si>
+  <si>
+    <t>{{contacts.phoneNumber}} {{contacts}:hide-block-if-empty}</t>
+  </si>
+  <si>
+    <t>Confidentiality notice {{hideConfNotice}:hide-block-if-empty}</t>
   </si>
   <si>
     <t>This file is intended only for the internal company usage.</t>
-  </si>
-  <si>
-    <t>Confidentiality notice {{hideConfNotice}:collapse:hide}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -441,64 +446,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D396324-6246-4275-ADEA-E8026C051904}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{98C06348-6561-561B-BBCE-16A51CD79A61}">
+      <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="21">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="B11" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed hide-if excel examples + images
</commit_message>
<xml_diff>
--- a/source/_static/files/document-generation/demos/conditionally-clear-cells-template.xlsx
+++ b/source/_static/files/document-generation/demos/conditionally-clear-cells-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PlumsailGit\TemplaterTest\Templater\bin\Debug\net461\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DocumentsDocs\source\_static\files\document-generation\demos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="10_ncr:100000_{68E69BE7-0B6D-4CC1-B158-F7BBC5A92F4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{D28C8233-CD5B-4A18-8C9B-6DE80ABA2AF8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{740EF94A-AB22-4470-A130-F6ADB22CB504}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{2A8C93E8-18E1-47EF-BD03-E7FC040C7E6E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2A8C93E8-18E1-47EF-BD03-E7FC040C7E6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,17 +59,17 @@
     <t>{{contacts.phoneNumber}} {{contacts}:hide-block-if-empty}</t>
   </si>
   <si>
-    <t>Confidentiality notice {{hideConfNotice}:hide-block-if-empty}</t>
-  </si>
-  <si>
     <t>This file is intended only for the internal company usage.</t>
+  </si>
+  <si>
+    <t>Confidentiality notice {{hideConfNotice}:hide-block-if(true)}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,22 +446,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D396324-6246-4275-ADEA-E8026C051904}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{98C06348-6561-561B-BBCE-16A51CD79A61}">
-      <selection activeCell="A9" sqref="A9:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -477,33 +477,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75">
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75">
+    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
     </row>
   </sheetData>

</xml_diff>